<commit_message>
updated a date error
</commit_message>
<xml_diff>
--- a/Supplemental_Files/SF3_ALS-CS-OptumClarity.xlsx
+++ b/Supplemental_Files/SF3_ALS-CS-OptumClarity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferwilson/Documents/network_drug_classes_als/Supplemental_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F861A1-2786-CF43-8CD7-87547C00FAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CE5F1B-3BAB-EF42-A0D6-EC580A117151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28620" yWindow="13360" windowWidth="26440" windowHeight="15440" activeTab="4" xr2:uid="{800572C8-76AA-EF4F-9361-1B5ED75BAB74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="4" xr2:uid="{800572C8-76AA-EF4F-9361-1B5ED75BAB74}"/>
   </bookViews>
   <sheets>
     <sheet name="TargTotPats" sheetId="1" r:id="rId1"/>
@@ -4895,7 +4895,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5046,7 +5046,7 @@
         <v>1918</v>
       </c>
       <c r="D16">
-        <v>1911</v>
+        <v>1991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>